<commit_message>
cleared the excel files
</commit_message>
<xml_diff>
--- a/src/excel graphs/graphoutput.xlsx
+++ b/src/excel graphs/graphoutput.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sunilv/Desktop/screenshots/learnings/plug-the-cli/src/excel graphs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{683DC085-33EB-2B4D-B8AA-71647A3756DF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7DC5CC86-64A8-CA44-A032-52A3D42D078A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1840" yWindow="860" windowWidth="31700" windowHeight="17440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1691,7 +1691,7 @@
   <dimension ref="C6:E25"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7:E7"/>
+      <selection activeCell="K33" sqref="K33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>